<commit_message>
include downpayment in expenses
</commit_message>
<xml_diff>
--- a/excel/2/1420 Terry - 3 - Add Expenses.xlsx
+++ b/excel/2/1420 Terry - 3 - Add Expenses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{6B2BACE4-D29B-AC4D-90BF-6B88B76DFC11}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{6B2BACE4-D29B-AC4D-90BF-6B88B76DFC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1338,7 +1338,7 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>-53626.34</c:v>
+                  <c:v>-68140.579999999987</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-26724.559999999998</c:v>
@@ -3109,8 +3109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C96533-4FC3-8F4F-BA09-1D518A28119D}">
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3207,7 +3207,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="5">
-        <v>-20137.46</v>
+        <v>-34651.699999999997</v>
       </c>
       <c r="I2" s="10">
         <f t="shared" ref="I2:I32" si="0">0.035/12</f>
@@ -3232,7 +3232,7 @@
       <c r="O2" s="11"/>
       <c r="P2" s="8">
         <f>12*(C2+D2+E2+F2+G2)+H2</f>
-        <v>-53626.34</v>
+        <v>-68140.579999999987</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
returns with new zillow estimate
</commit_message>
<xml_diff>
--- a/excel/2/1420 Terry - 3 - Add Expenses.xlsx
+++ b/excel/2/1420 Terry - 3 - Add Expenses.xlsx
@@ -59,9 +59,6 @@
     <t>PMI Payment</t>
   </si>
   <si>
-    <t>Δ Equity</t>
-  </si>
-  <si>
     <t>Rent</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>Escrow Payment</t>
+  </si>
+  <si>
+    <t>Δ Equity + Expenses</t>
   </si>
 </sst>
 </file>
@@ -145,7 +145,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -161,6 +161,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3109,8 +3110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C96533-4FC3-8F4F-BA09-1D518A28119D}">
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3126,7 +3127,7 @@
     <col min="11" max="11" width="13.6640625" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
     <col min="13" max="13" width="14.83203125" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="18" customWidth="1"/>
     <col min="15" max="15" width="14.1640625" customWidth="1"/>
     <col min="16" max="16" width="13.6640625" customWidth="1"/>
     <col min="17" max="17" width="12.1640625" customWidth="1"/>
@@ -3146,16 +3147,16 @@
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
@@ -3172,14 +3173,14 @@
       <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>11</v>
+      <c r="N1" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q1" s="14"/>
     </row>

</xml_diff>

<commit_message>
revise model and compute return
</commit_message>
<xml_diff>
--- a/excel/2/1420 Terry - 3 - Add Expenses.xlsx
+++ b/excel/2/1420 Terry - 3 - Add Expenses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{6B2BACE4-D29B-AC4D-90BF-6B88B76DFC11}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{6B2BACE4-D29B-AC4D-90BF-6B88B76DFC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -736,19 +736,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="1">
-                  <c:v>-2.5843668846901857</c:v>
+                  <c:v>-1.1385657125128108</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.16736907397995762</c:v>
+                  <c:v>0.24227133967349268</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8.8827021220126673E-2</c:v>
+                  <c:v>0.17246077401921209</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.1394974536227695</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.15249320839109795</c:v>
+                  <c:v>8.2995144086756859E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>9.3780624765330042E-2</c:v>
@@ -3110,8 +3110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C96533-4FC3-8F4F-BA09-1D518A28119D}">
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="M24" zoomScale="101" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3285,12 +3285,12 @@
         <v>25471.510261746647</v>
       </c>
       <c r="N3" s="8">
-        <f>M3-M2+12*(C3+D3+E3+F3+G3+H3)</f>
-        <v>-23370.429738253348</v>
+        <f>M3-M2+12*(C3+D3+E3+F3+G3)+H3</f>
+        <v>-10296.049738253349</v>
       </c>
       <c r="O3" s="13">
         <f>N3/M2</f>
-        <v>-2.5843668846901857</v>
+        <v>-1.1385657125128108</v>
       </c>
       <c r="P3" s="8">
         <f t="shared" ref="P3:P66" si="5">12*(C3+D3+E3+F3+G3)+H3</f>
@@ -3346,12 +3346,12 @@
         <v>42427.967176367121</v>
       </c>
       <c r="N4" s="8">
-        <f t="shared" ref="N4:N67" si="6">M4-M3+12*(C4+D4+E4+F4+G4+H4)</f>
-        <v>-4263.1430853795246</v>
+        <f t="shared" ref="N4:N67" si="6">M4-M3+12*(C4+D4+E4+F4+G4)+H4</f>
+        <v>6171.0169146204762</v>
       </c>
       <c r="O4" s="13">
         <f t="shared" ref="O4:O67" si="7">N4/M3</f>
-        <v>-0.16736907397995762</v>
+        <v>0.24227133967349268</v>
       </c>
       <c r="P4" s="8">
         <f t="shared" si="5"/>
@@ -3408,11 +3408,11 @@
       </c>
       <c r="N5" s="8">
         <f t="shared" si="6"/>
-        <v>-3768.7499407020005</v>
+        <v>7317.1600592979976</v>
       </c>
       <c r="O5" s="13">
         <f t="shared" si="7"/>
-        <v>-8.8827021220126673E-2</v>
+        <v>0.17246077401921209</v>
       </c>
       <c r="P5" s="8">
         <f t="shared" si="5"/>
@@ -3528,11 +3528,11 @@
       </c>
       <c r="N7" s="8">
         <f t="shared" si="6"/>
-        <v>-11893.497945157349</v>
+        <v>6473.0920548426511</v>
       </c>
       <c r="O7" s="13">
         <f t="shared" si="7"/>
-        <v>-0.15249320839109795</v>
+        <v>8.2995144086756859E-2</v>
       </c>
       <c r="P7" s="8">
         <f t="shared" si="5"/>
@@ -7010,7 +7010,7 @@
         <v>2374272.7481103335</v>
       </c>
       <c r="N68" s="8">
-        <f t="shared" ref="N68:N71" si="18">M68-M67+12*(C68+D68+E68+F68+G68+H68)</f>
+        <f t="shared" ref="N68:N71" si="18">M68-M67+12*(C68+D68+E68+F68+G68)+H68</f>
         <v>133952.64294126967</v>
       </c>
       <c r="O68" s="13">

</xml_diff>